<commit_message>
updating mapping sheets and samples
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Person Health_Information_Search_Request/artifacts/service_model/information_model/IEPD/documentation/mapping.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Person Health_Information_Search_Request/artifacts/service_model/information_model/IEPD/documentation/mapping.xlsx
@@ -63,43 +63,43 @@
     <t>Gender</t>
   </si>
   <si>
-    <t>/evalsr-doc:PersonEvaluationSearchRequest/nc30:Person/nc30:PersonName/nc30:PersonGivenName</t>
-  </si>
-  <si>
-    <t>/evalsr-doc:PersonEvaluationSearchRequest/nc30:Person/nc30:PersonName/nc30:PersonMiddleName</t>
-  </si>
-  <si>
-    <t>/evalsr-doc:PersonEvaluationSearchRequest/nc30:Person/nc30:PersonName/nc30:PersonSurName</t>
-  </si>
-  <si>
-    <t>/evalsr-doc:PersonEvaluationSearchRequest/nc30:Person/nc30:PersonBirthDate/nc30:Date</t>
-  </si>
-  <si>
-    <t>/evalsr-doc:PersonEvaluationSearchRequest/nc30:Person/jxdm51:PersonRaceCode</t>
-  </si>
-  <si>
-    <t>/evalsr-doc:PersonEvaluationSearchRequest/nc30:Person/jxdm51:PersonEthnicityCode</t>
-  </si>
-  <si>
-    <t>/evalsr-doc:PersonEvaluationSearchRequest/nc30:Person/jxdm51:PersonSexCode</t>
-  </si>
-  <si>
-    <t>/evalsr-doc:PersonEvaluationSearchRequest/nc30:Person/evalsr-ext:PersonTemporaryIdentification/nc30:IdentificationID</t>
-  </si>
-  <si>
-    <t>/evalsr-doc:PersonEvaluationSearchRequest/nc30:Identity[@structures:id=/evalsr-doc:PersonEvaluationSearchRequest/nc30:PersonAliasIdentityAssociation[nc30:Person/@structures:ref=/evalsr-doc:PersonEvaluationSearchRequest/nc30:Person/@structures:id]/nc30:Identity/@structures:ref]/nc30:IdentityPersonRepresentation/nc30:PersonName/nc30:PersonGivenName</t>
-  </si>
-  <si>
-    <t>/evalsr-doc:PersonEvaluationSearchRequest/nc30:Identity[@structures:id=/evalsr-doc:PersonEvaluationSearchRequest/nc30:PersonAliasIdentityAssociation[nc30:Person/@structures:ref=/evalsr-doc:PersonEvaluationSearchRequest/nc30:Person/@structures:id]/nc30:Identity/@structures:ref]/nc30:IdentityPersonRepresentation/nc30:PersonName/nc30:PersonMiddleName</t>
-  </si>
-  <si>
-    <t>/evalsr-doc:PersonEvaluationSearchRequest/nc30:Identity[@structures:id=/evalsr-doc:PersonEvaluationSearchRequest/nc30:PersonAliasIdentityAssociation[nc30:Person/@structures:ref=/evalsr-doc:PersonEvaluationSearchRequest/nc30:Person/@structures:id]/nc30:Identity/@structures:ref]/nc30:IdentityPersonRepresentation/nc30:PersonName/nc30:PersonSurName</t>
-  </si>
-  <si>
-    <t>/evalsr-doc:PersonEvaluationSearchRequest/nc30:Identity[@structures:id=/evalsr-doc:PersonEvaluationSearchRequest/nc30:PersonAliasIdentityAssociation[nc30:Person/@structures:ref=/evalsr-doc:PersonEvaluationSearchRequest/nc30:Person/@structures:id]/nc30:Identity/@structures:ref]/nc30:IdentityPersonRepresentation/nc30:PersonBirthDate/nc30:Date</t>
-  </si>
-  <si>
-    <t>/evalsr-doc:PersonEvaluationSearchRequest/nc30:Identity[@structures:id=/evalsr-doc:PersonEvaluationSearchRequest/nc30:PersonAliasIdentityAssociation[nc30:Person/@structures:ref=/evalsr-doc:PersonEvaluationSearchRequest/nc30:Person/@structures:id]/nc30:Identity/@structures:ref]/nc30:IdentityPersonRepresentation/jxdm51:PersonSexCode</t>
+    <t>/phisr-doc:PersonHealthInformationSearchRequest/nc30:Person/nc30:PersonName/nc30:PersonGivenName</t>
+  </si>
+  <si>
+    <t>/phisr-doc:PersonHealthInformationSearchRequest/nc30:Person/nc30:PersonName/nc30:PersonMiddleName</t>
+  </si>
+  <si>
+    <t>/phisr-doc:PersonHealthInformationSearchRequest/nc30:Person/nc30:PersonName/nc30:PersonSurName</t>
+  </si>
+  <si>
+    <t>/phisr-doc:PersonHealthInformationSearchRequest/nc30:Person/nc30:PersonBirthDate/nc30:Date</t>
+  </si>
+  <si>
+    <t>/phisr-doc:PersonHealthInformationSearchRequest/nc30:Person/jxdm51:PersonRaceCode</t>
+  </si>
+  <si>
+    <t>/phisr-doc:PersonHealthInformationSearchRequest/nc30:Person/jxdm51:PersonEthnicityCode</t>
+  </si>
+  <si>
+    <t>/phisr-doc:PersonHealthInformationSearchRequest/nc30:Person/jxdm51:PersonSexCode</t>
+  </si>
+  <si>
+    <t>/phisr-doc:PersonHealthInformationSearchRequest/nc30:Person/phisr-ext:PersonTemporaryIdentification/nc30:IdentificationID</t>
+  </si>
+  <si>
+    <t>/phisr-doc:PersonHealthInformationSearchRequest/nc30:Identity[@structures:id=/phisr-doc:PersonHealthInformationSearchRequest/nc30:PersonAliasIdentityAssociation[nc30:Person/@structures:ref=/phisr-doc:PersonHealthInformationSearchRequest/nc30:Person/@structures:id]/nc30:Identity/@structures:ref]/nc30:IdentityPersonRepresentation/nc30:PersonName/nc30:PersonGivenName</t>
+  </si>
+  <si>
+    <t>/phisr-doc:PersonHealthInformationSearchRequest/nc30:Identity[@structures:id=/phisr-doc:PersonHealthInformationSearchRequest/nc30:PersonAliasIdentityAssociation[nc30:Person/@structures:ref=/phisr-doc:PersonHealthInformationSearchRequest/nc30:Person/@structures:id]/nc30:Identity/@structures:ref]/nc30:IdentityPersonRepresentation/nc30:PersonName/nc30:PersonMiddleName</t>
+  </si>
+  <si>
+    <t>/phisr-doc:PersonHealthInformationSearchRequest/nc30:Identity[@structures:id=/phisr-doc:PersonHealthInformationSearchRequest/nc30:PersonAliasIdentityAssociation[nc30:Person/@structures:ref=/phisr-doc:PersonHealthInformationSearchRequest/nc30:Person/@structures:id]/nc30:Identity/@structures:ref]/nc30:IdentityPersonRepresentation/nc30:PersonName/nc30:PersonSurName</t>
+  </si>
+  <si>
+    <t>/phisr-doc:PersonHealthInformationSearchRequest/nc30:Identity[@structures:id=/phisr-doc:PersonHealthInformationSearchRequest/nc30:PersonAliasIdentityAssociation[nc30:Person/@structures:ref=/phisr-doc:PersonHealthInformationSearchRequest/nc30:Person/@structures:id]/nc30:Identity/@structures:ref]/nc30:IdentityPersonRepresentation/nc30:PersonBirthDate/nc30:Date</t>
+  </si>
+  <si>
+    <t>/phisr-doc:PersonHealthInformationSearchRequest/nc30:Identity[@structures:id=/phisr-doc:PersonHealthInformationSearchRequest/nc30:PersonAliasIdentityAssociation[nc30:Person/@structures:ref=/phisr-doc:PersonHealthInformationSearchRequest/nc30:Person/@structures:id]/nc30:Identity/@structures:ref]/nc30:IdentityPersonRepresentation/jxdm51:PersonSexCode</t>
   </si>
 </sst>
 </file>
@@ -552,7 +552,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>